<commit_message>
feat: update scripts actions and style of emails
</commit_message>
<xml_diff>
--- a/func.xlsx
+++ b/func.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sn1082087\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sn1082087\Desktop\ssi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{706CBD15-8C58-420C-8AD3-0539C1096C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9558C831-4538-4255-8C15-19185A3A6DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1E4BCFC-6CFF-4140-AF51-69E49F4332DA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -50,12 +50,6 @@
     <t>areaCode</t>
   </si>
   <si>
-    <t>João Silva</t>
-  </si>
-  <si>
-    <t>joao.silva@sp.senai.br</t>
-  </si>
-  <si>
     <t>COMMON</t>
   </si>
   <si>
@@ -66,6 +60,24 @@
   </si>
   <si>
     <t>TECHNICIAN</t>
+  </si>
+  <si>
+    <t>Vitor Rios</t>
+  </si>
+  <si>
+    <t>vitor.rios@sp.senai.br</t>
+  </si>
+  <si>
+    <t>Augusto Atanasio</t>
+  </si>
+  <si>
+    <t>augusto.atanasio@sp.senai.br</t>
+  </si>
+  <si>
+    <t>Maria Messias</t>
+  </si>
+  <si>
+    <t>maria.messias@sp.senai.br</t>
   </si>
 </sst>
 </file>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371B6E24-E669-4F2B-A946-F986EB9756A7}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,30 +488,54 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{26CF9D09-15CB-4EFB-9D6F-1623980D6A3C}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{8BD8DE89-5C69-4340-9F40-A55C5F84FCD2}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{4EE30FB9-9A43-4BFA-B219-4BD430A4F716}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{024936F1-3625-4DC3-9FD1-4D6D2F6FA3FD}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>